<commit_message>
There was one more line in the header and removed this for processing.
</commit_message>
<xml_diff>
--- a/20140604_emd/경상북도/읍면동별 개표자료-02_구시군장-포항시-02 포항시남구.xlsx
+++ b/20140604_emd/경상북도/읍면동별 개표자료-02_구시군장-포항시-02 포항시남구.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="17400" windowHeight="12495"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="17400" windowHeight="12500"/>
   </bookViews>
   <sheets>
     <sheet name="포항시장(포항시남구)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="41">
   <si>
     <t>읍면동명</t>
   </si>
@@ -32,9 +37,6 @@
   <si>
     <t>새누리당
 이강덕</t>
-  </si>
-  <si>
-    <t>후 보 자 별 득 표 수</t>
   </si>
   <si>
     <t>유 효 투 표 수 (가)</t>
@@ -158,22 +160,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -181,7 +183,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -190,7 +192,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -204,14 +206,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -220,7 +222,7 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -240,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -250,29 +252,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -280,60 +282,49 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -357,11 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -383,7 +374,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -398,15 +389,19 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -416,19 +411,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -444,14 +431,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -742,22 +725,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="13.125" style="4" customWidth="1"/>
-    <col min="3" max="11" width="13.125" customWidth="1"/>
+    <col min="1" max="2" width="13.1640625" style="4" customWidth="1"/>
+    <col min="3" max="11" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="23">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -773,11 +756,11 @@
     <row r="2" spans="1:11" ht="13.5" customHeight="1"/>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
@@ -787,132 +770,152 @@
       <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="14" t="s">
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="38.25" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="8" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="13">
+        <v>201120</v>
+      </c>
+      <c r="D6" s="13">
+        <v>103003</v>
+      </c>
+      <c r="E6" s="13">
+        <v>69752</v>
+      </c>
+      <c r="F6" s="13">
+        <v>14406</v>
+      </c>
+      <c r="G6" s="13">
+        <v>16909</v>
+      </c>
+      <c r="H6" s="13">
+        <v>101067</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1936</v>
+      </c>
+      <c r="J6" s="13">
+        <v>98117</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="13">
-        <v>201120</v>
-      </c>
-      <c r="D7" s="13">
-        <v>103003</v>
-      </c>
-      <c r="E7" s="13">
-        <v>69752</v>
-      </c>
-      <c r="F7" s="13">
-        <v>14406</v>
-      </c>
-      <c r="G7" s="13">
-        <v>16909</v>
-      </c>
-      <c r="H7" s="13">
-        <v>101067</v>
-      </c>
-      <c r="I7" s="13">
-        <v>1936</v>
-      </c>
-      <c r="J7" s="13">
-        <v>98117</v>
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11">
+        <v>564</v>
+      </c>
+      <c r="D7" s="11">
+        <v>518</v>
+      </c>
+      <c r="E7" s="11">
+        <v>347</v>
+      </c>
+      <c r="F7" s="11">
+        <v>74</v>
+      </c>
+      <c r="G7" s="11">
+        <v>72</v>
+      </c>
+      <c r="H7" s="11">
+        <v>493</v>
+      </c>
+      <c r="I7" s="11">
+        <v>25</v>
+      </c>
+      <c r="J7" s="11">
+        <v>46</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" s="11">
-        <v>564</v>
+        <v>8379</v>
       </c>
       <c r="D8" s="11">
-        <v>518</v>
+        <v>8379</v>
       </c>
       <c r="E8" s="11">
-        <v>347</v>
+        <v>5007</v>
       </c>
       <c r="F8" s="11">
-        <v>74</v>
+        <v>1833</v>
       </c>
       <c r="G8" s="11">
-        <v>72</v>
+        <v>1372</v>
       </c>
       <c r="H8" s="11">
-        <v>493</v>
+        <v>8212</v>
       </c>
       <c r="I8" s="11">
-        <v>25</v>
+        <v>167</v>
       </c>
       <c r="J8" s="11">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -920,209 +923,209 @@
         <v>16</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11">
-        <v>8379</v>
+        <v>8311</v>
       </c>
       <c r="D9" s="11">
-        <v>8379</v>
+        <v>4969</v>
       </c>
       <c r="E9" s="11">
-        <v>5007</v>
+        <v>3913</v>
       </c>
       <c r="F9" s="11">
-        <v>1833</v>
+        <v>317</v>
       </c>
       <c r="G9" s="11">
-        <v>1372</v>
+        <v>554</v>
       </c>
       <c r="H9" s="11">
-        <v>8212</v>
+        <v>4784</v>
       </c>
       <c r="I9" s="11">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="J9" s="11">
-        <v>0</v>
+        <v>3342</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" s="11">
-        <v>8311</v>
+        <v>868</v>
       </c>
       <c r="D10" s="11">
-        <v>4969</v>
+        <v>868</v>
       </c>
       <c r="E10" s="11">
-        <v>3913</v>
+        <v>664</v>
       </c>
       <c r="F10" s="11">
-        <v>317</v>
+        <v>64</v>
       </c>
       <c r="G10" s="11">
-        <v>554</v>
+        <v>91</v>
       </c>
       <c r="H10" s="11">
-        <v>4784</v>
+        <v>819</v>
       </c>
       <c r="I10" s="11">
-        <v>185</v>
+        <v>49</v>
       </c>
       <c r="J10" s="11">
-        <v>3342</v>
+        <v>0</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="11">
-        <v>868</v>
+        <v>7443</v>
       </c>
       <c r="D11" s="11">
-        <v>868</v>
+        <v>4101</v>
       </c>
       <c r="E11" s="11">
-        <v>664</v>
+        <v>3249</v>
       </c>
       <c r="F11" s="11">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="G11" s="11">
-        <v>91</v>
+        <v>463</v>
       </c>
       <c r="H11" s="11">
-        <v>819</v>
+        <v>3965</v>
       </c>
       <c r="I11" s="11">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="J11" s="11">
-        <v>0</v>
+        <v>3342</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C12" s="11">
-        <v>7443</v>
+        <v>25138</v>
       </c>
       <c r="D12" s="11">
-        <v>4101</v>
+        <v>12240</v>
       </c>
       <c r="E12" s="11">
-        <v>3249</v>
+        <v>8184</v>
       </c>
       <c r="F12" s="11">
-        <v>253</v>
+        <v>1667</v>
       </c>
       <c r="G12" s="11">
-        <v>463</v>
+        <v>2223</v>
       </c>
       <c r="H12" s="11">
-        <v>3965</v>
+        <v>12074</v>
       </c>
       <c r="I12" s="11">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="J12" s="11">
-        <v>3342</v>
+        <v>12898</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C13" s="11">
-        <v>25138</v>
+        <v>1385</v>
       </c>
       <c r="D13" s="11">
-        <v>12240</v>
+        <v>1384</v>
       </c>
       <c r="E13" s="11">
-        <v>8184</v>
+        <v>903</v>
       </c>
       <c r="F13" s="11">
-        <v>1667</v>
+        <v>218</v>
       </c>
       <c r="G13" s="11">
-        <v>2223</v>
+        <v>241</v>
       </c>
       <c r="H13" s="11">
-        <v>12074</v>
+        <v>1362</v>
       </c>
       <c r="I13" s="11">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="J13" s="11">
-        <v>12898</v>
+        <v>1</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="11">
-        <v>1385</v>
+        <v>23753</v>
       </c>
       <c r="D14" s="11">
-        <v>1384</v>
+        <v>10856</v>
       </c>
       <c r="E14" s="11">
-        <v>903</v>
+        <v>7281</v>
       </c>
       <c r="F14" s="11">
-        <v>218</v>
+        <v>1449</v>
       </c>
       <c r="G14" s="11">
-        <v>241</v>
+        <v>1982</v>
       </c>
       <c r="H14" s="11">
-        <v>1362</v>
+        <v>10712</v>
       </c>
       <c r="I14" s="11">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="J14" s="11">
-        <v>1</v>
+        <v>12897</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1130,104 +1133,104 @@
         <v>20</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C15" s="11">
-        <v>23753</v>
+        <v>38116</v>
       </c>
       <c r="D15" s="11">
-        <v>10856</v>
+        <v>16477</v>
       </c>
       <c r="E15" s="11">
-        <v>7281</v>
+        <v>10831</v>
       </c>
       <c r="F15" s="11">
-        <v>1449</v>
+        <v>2592</v>
       </c>
       <c r="G15" s="11">
-        <v>1982</v>
+        <v>2737</v>
       </c>
       <c r="H15" s="11">
-        <v>10712</v>
+        <v>16160</v>
       </c>
       <c r="I15" s="11">
-        <v>144</v>
+        <v>317</v>
       </c>
       <c r="J15" s="11">
-        <v>12897</v>
+        <v>21639</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C16" s="11">
-        <v>38116</v>
+        <v>2268</v>
       </c>
       <c r="D16" s="11">
-        <v>16477</v>
+        <v>2266</v>
       </c>
       <c r="E16" s="11">
-        <v>10831</v>
+        <v>1465</v>
       </c>
       <c r="F16" s="11">
-        <v>2592</v>
+        <v>385</v>
       </c>
       <c r="G16" s="11">
-        <v>2737</v>
+        <v>366</v>
       </c>
       <c r="H16" s="11">
-        <v>16160</v>
+        <v>2216</v>
       </c>
       <c r="I16" s="11">
-        <v>317</v>
+        <v>50</v>
       </c>
       <c r="J16" s="11">
-        <v>21639</v>
+        <v>2</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="11">
-        <v>2268</v>
+        <v>35848</v>
       </c>
       <c r="D17" s="11">
-        <v>2266</v>
+        <v>14211</v>
       </c>
       <c r="E17" s="11">
-        <v>1465</v>
+        <v>9366</v>
       </c>
       <c r="F17" s="11">
-        <v>385</v>
+        <v>2207</v>
       </c>
       <c r="G17" s="11">
-        <v>366</v>
+        <v>2371</v>
       </c>
       <c r="H17" s="11">
-        <v>2216</v>
+        <v>13944</v>
       </c>
       <c r="I17" s="11">
-        <v>50</v>
+        <v>267</v>
       </c>
       <c r="J17" s="11">
-        <v>2</v>
+        <v>21637</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1235,104 +1238,104 @@
         <v>21</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C18" s="11">
-        <v>35848</v>
+        <v>4116</v>
       </c>
       <c r="D18" s="11">
-        <v>14211</v>
+        <v>2377</v>
       </c>
       <c r="E18" s="11">
-        <v>9366</v>
+        <v>1720</v>
       </c>
       <c r="F18" s="11">
-        <v>2207</v>
+        <v>218</v>
       </c>
       <c r="G18" s="11">
-        <v>2371</v>
+        <v>368</v>
       </c>
       <c r="H18" s="11">
-        <v>13944</v>
+        <v>2306</v>
       </c>
       <c r="I18" s="11">
-        <v>267</v>
+        <v>71</v>
       </c>
       <c r="J18" s="11">
-        <v>21637</v>
+        <v>1739</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C19" s="11">
-        <v>4116</v>
+        <v>314</v>
       </c>
       <c r="D19" s="11">
-        <v>2377</v>
+        <v>314</v>
       </c>
       <c r="E19" s="11">
-        <v>1720</v>
+        <v>246</v>
       </c>
       <c r="F19" s="11">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="G19" s="11">
-        <v>368</v>
+        <v>39</v>
       </c>
       <c r="H19" s="11">
-        <v>2306</v>
+        <v>302</v>
       </c>
       <c r="I19" s="11">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="J19" s="11">
-        <v>1739</v>
+        <v>0</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11">
-        <v>314</v>
+        <v>3802</v>
       </c>
       <c r="D20" s="11">
-        <v>314</v>
+        <v>2063</v>
       </c>
       <c r="E20" s="11">
-        <v>246</v>
+        <v>1474</v>
       </c>
       <c r="F20" s="11">
-        <v>17</v>
+        <v>201</v>
       </c>
       <c r="G20" s="11">
-        <v>39</v>
+        <v>329</v>
       </c>
       <c r="H20" s="11">
-        <v>302</v>
+        <v>2004</v>
       </c>
       <c r="I20" s="11">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="J20" s="11">
-        <v>0</v>
+        <v>1739</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1340,104 +1343,104 @@
         <v>22</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11">
-        <v>3802</v>
+        <v>8638</v>
       </c>
       <c r="D21" s="11">
-        <v>2063</v>
+        <v>4918</v>
       </c>
       <c r="E21" s="11">
-        <v>1474</v>
+        <v>3583</v>
       </c>
       <c r="F21" s="11">
-        <v>201</v>
+        <v>586</v>
       </c>
       <c r="G21" s="11">
-        <v>329</v>
+        <v>612</v>
       </c>
       <c r="H21" s="11">
-        <v>2004</v>
+        <v>4781</v>
       </c>
       <c r="I21" s="11">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="J21" s="11">
-        <v>1739</v>
+        <v>3720</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C22" s="11">
-        <v>8638</v>
+        <v>958</v>
       </c>
       <c r="D22" s="11">
-        <v>4918</v>
+        <v>956</v>
       </c>
       <c r="E22" s="11">
-        <v>3583</v>
+        <v>672</v>
       </c>
       <c r="F22" s="11">
-        <v>586</v>
+        <v>123</v>
       </c>
       <c r="G22" s="11">
-        <v>612</v>
+        <v>120</v>
       </c>
       <c r="H22" s="11">
-        <v>4781</v>
+        <v>915</v>
       </c>
       <c r="I22" s="11">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="J22" s="11">
-        <v>3720</v>
+        <v>2</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="11">
-        <v>958</v>
+        <v>7680</v>
       </c>
       <c r="D23" s="11">
-        <v>956</v>
+        <v>3962</v>
       </c>
       <c r="E23" s="11">
-        <v>672</v>
+        <v>2911</v>
       </c>
       <c r="F23" s="11">
-        <v>123</v>
+        <v>463</v>
       </c>
       <c r="G23" s="11">
-        <v>120</v>
+        <v>492</v>
       </c>
       <c r="H23" s="11">
-        <v>915</v>
+        <v>3866</v>
       </c>
       <c r="I23" s="11">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="J23" s="11">
-        <v>2</v>
+        <v>3718</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1445,104 +1448,104 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C24" s="11">
-        <v>7680</v>
+        <v>4362</v>
       </c>
       <c r="D24" s="11">
-        <v>3962</v>
+        <v>2675</v>
       </c>
       <c r="E24" s="11">
-        <v>2911</v>
+        <v>2351</v>
       </c>
       <c r="F24" s="11">
-        <v>463</v>
+        <v>95</v>
       </c>
       <c r="G24" s="11">
-        <v>492</v>
+        <v>127</v>
       </c>
       <c r="H24" s="11">
-        <v>3866</v>
+        <v>2573</v>
       </c>
       <c r="I24" s="11">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="J24" s="11">
-        <v>3718</v>
+        <v>1687</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C25" s="11">
-        <v>4362</v>
+        <v>560</v>
       </c>
       <c r="D25" s="11">
-        <v>2675</v>
+        <v>560</v>
       </c>
       <c r="E25" s="11">
-        <v>2351</v>
+        <v>498</v>
       </c>
       <c r="F25" s="11">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="G25" s="11">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="H25" s="11">
-        <v>2573</v>
+        <v>538</v>
       </c>
       <c r="I25" s="11">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="J25" s="11">
-        <v>1687</v>
+        <v>0</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="11">
-        <v>560</v>
+        <v>3802</v>
       </c>
       <c r="D26" s="11">
-        <v>560</v>
+        <v>2115</v>
       </c>
       <c r="E26" s="11">
-        <v>498</v>
+        <v>1853</v>
       </c>
       <c r="F26" s="11">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="G26" s="11">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="H26" s="11">
-        <v>538</v>
+        <v>2035</v>
       </c>
       <c r="I26" s="11">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="J26" s="11">
-        <v>0</v>
+        <v>1687</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1550,104 +1553,104 @@
         <v>24</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11">
-        <v>3802</v>
+        <v>2014</v>
       </c>
       <c r="D27" s="11">
-        <v>2115</v>
+        <v>1295</v>
       </c>
       <c r="E27" s="11">
-        <v>1853</v>
+        <v>1055</v>
       </c>
       <c r="F27" s="11">
+        <v>63</v>
+      </c>
+      <c r="G27" s="11">
+        <v>107</v>
+      </c>
+      <c r="H27" s="11">
+        <v>1225</v>
+      </c>
+      <c r="I27" s="11">
         <v>70</v>
       </c>
-      <c r="G27" s="11">
-        <v>112</v>
-      </c>
-      <c r="H27" s="11">
-        <v>2035</v>
-      </c>
-      <c r="I27" s="11">
-        <v>80</v>
-      </c>
       <c r="J27" s="11">
-        <v>1687</v>
+        <v>719</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C28" s="11">
-        <v>2014</v>
+        <v>274</v>
       </c>
       <c r="D28" s="11">
-        <v>1295</v>
+        <v>274</v>
       </c>
       <c r="E28" s="11">
-        <v>1055</v>
+        <v>223</v>
       </c>
       <c r="F28" s="11">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="G28" s="11">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="H28" s="11">
-        <v>1225</v>
+        <v>254</v>
       </c>
       <c r="I28" s="11">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="J28" s="11">
-        <v>719</v>
+        <v>0</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="11">
-        <v>274</v>
+        <v>1740</v>
       </c>
       <c r="D29" s="11">
-        <v>274</v>
+        <v>1021</v>
       </c>
       <c r="E29" s="11">
-        <v>223</v>
+        <v>832</v>
       </c>
       <c r="F29" s="11">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="G29" s="11">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="H29" s="11">
-        <v>254</v>
+        <v>971</v>
       </c>
       <c r="I29" s="11">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J29" s="11">
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1655,104 +1658,104 @@
         <v>25</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C30" s="11">
-        <v>1740</v>
+        <v>23359</v>
       </c>
       <c r="D30" s="11">
-        <v>1021</v>
+        <v>10622</v>
       </c>
       <c r="E30" s="11">
-        <v>832</v>
+        <v>7612</v>
       </c>
       <c r="F30" s="11">
-        <v>53</v>
+        <v>1087</v>
       </c>
       <c r="G30" s="11">
-        <v>86</v>
+        <v>1795</v>
       </c>
       <c r="H30" s="11">
-        <v>971</v>
+        <v>10494</v>
       </c>
       <c r="I30" s="11">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="J30" s="11">
-        <v>719</v>
+        <v>12737</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C31" s="11">
-        <v>23359</v>
+        <v>1090</v>
       </c>
       <c r="D31" s="11">
-        <v>10622</v>
+        <v>1090</v>
       </c>
       <c r="E31" s="11">
-        <v>7612</v>
+        <v>721</v>
       </c>
       <c r="F31" s="11">
-        <v>1087</v>
+        <v>157</v>
       </c>
       <c r="G31" s="11">
-        <v>1795</v>
+        <v>193</v>
       </c>
       <c r="H31" s="11">
-        <v>10494</v>
+        <v>1071</v>
       </c>
       <c r="I31" s="11">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="J31" s="11">
-        <v>12737</v>
+        <v>0</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="11">
-        <v>1090</v>
+        <v>22269</v>
       </c>
       <c r="D32" s="11">
-        <v>1090</v>
+        <v>9532</v>
       </c>
       <c r="E32" s="11">
-        <v>721</v>
+        <v>6891</v>
       </c>
       <c r="F32" s="11">
-        <v>157</v>
+        <v>930</v>
       </c>
       <c r="G32" s="11">
-        <v>193</v>
+        <v>1602</v>
       </c>
       <c r="H32" s="11">
-        <v>1071</v>
+        <v>9423</v>
       </c>
       <c r="I32" s="11">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="J32" s="11">
-        <v>0</v>
+        <v>12737</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1760,104 +1763,104 @@
         <v>26</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C33" s="11">
-        <v>22269</v>
+        <v>18148</v>
       </c>
       <c r="D33" s="11">
-        <v>9532</v>
+        <v>8055</v>
       </c>
       <c r="E33" s="11">
-        <v>6891</v>
+        <v>5883</v>
       </c>
       <c r="F33" s="11">
-        <v>930</v>
+        <v>738</v>
       </c>
       <c r="G33" s="11">
-        <v>1602</v>
+        <v>1302</v>
       </c>
       <c r="H33" s="11">
-        <v>9423</v>
+        <v>7923</v>
       </c>
       <c r="I33" s="11">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="J33" s="11">
-        <v>12737</v>
+        <v>10093</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C34" s="11">
-        <v>18148</v>
+        <v>826</v>
       </c>
       <c r="D34" s="11">
-        <v>8055</v>
+        <v>826</v>
       </c>
       <c r="E34" s="11">
-        <v>5883</v>
+        <v>595</v>
       </c>
       <c r="F34" s="11">
-        <v>738</v>
+        <v>85</v>
       </c>
       <c r="G34" s="11">
-        <v>1302</v>
+        <v>129</v>
       </c>
       <c r="H34" s="11">
-        <v>7923</v>
+        <v>809</v>
       </c>
       <c r="I34" s="11">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="J34" s="11">
-        <v>10093</v>
+        <v>0</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="11">
-        <v>826</v>
+        <v>17322</v>
       </c>
       <c r="D35" s="11">
-        <v>826</v>
+        <v>7229</v>
       </c>
       <c r="E35" s="11">
-        <v>595</v>
+        <v>5288</v>
       </c>
       <c r="F35" s="11">
-        <v>85</v>
+        <v>653</v>
       </c>
       <c r="G35" s="11">
-        <v>129</v>
+        <v>1173</v>
       </c>
       <c r="H35" s="11">
-        <v>809</v>
+        <v>7114</v>
       </c>
       <c r="I35" s="11">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="J35" s="11">
-        <v>0</v>
+        <v>10093</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1865,104 +1868,104 @@
         <v>27</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C36" s="11">
-        <v>17322</v>
+        <v>14046</v>
       </c>
       <c r="D36" s="11">
-        <v>7229</v>
+        <v>6752</v>
       </c>
       <c r="E36" s="11">
-        <v>5288</v>
+        <v>4994</v>
       </c>
       <c r="F36" s="11">
-        <v>653</v>
+        <v>557</v>
       </c>
       <c r="G36" s="11">
-        <v>1173</v>
+        <v>1080</v>
       </c>
       <c r="H36" s="11">
-        <v>7114</v>
+        <v>6631</v>
       </c>
       <c r="I36" s="11">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="J36" s="11">
-        <v>10093</v>
+        <v>7294</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C37" s="11">
-        <v>14046</v>
+        <v>1080</v>
       </c>
       <c r="D37" s="11">
-        <v>6752</v>
+        <v>1079</v>
       </c>
       <c r="E37" s="11">
-        <v>4994</v>
+        <v>799</v>
       </c>
       <c r="F37" s="11">
-        <v>557</v>
+        <v>86</v>
       </c>
       <c r="G37" s="11">
-        <v>1080</v>
+        <v>174</v>
       </c>
       <c r="H37" s="11">
-        <v>6631</v>
+        <v>1059</v>
       </c>
       <c r="I37" s="11">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="J37" s="11">
-        <v>7294</v>
+        <v>1</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="11">
-        <v>1080</v>
+        <v>12966</v>
       </c>
       <c r="D38" s="11">
-        <v>1079</v>
+        <v>5673</v>
       </c>
       <c r="E38" s="11">
-        <v>799</v>
+        <v>4195</v>
       </c>
       <c r="F38" s="11">
-        <v>86</v>
+        <v>471</v>
       </c>
       <c r="G38" s="11">
-        <v>174</v>
+        <v>906</v>
       </c>
       <c r="H38" s="11">
-        <v>1059</v>
+        <v>5572</v>
       </c>
       <c r="I38" s="11">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="J38" s="11">
-        <v>1</v>
+        <v>7293</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1970,104 +1973,104 @@
         <v>28</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C39" s="11">
-        <v>12966</v>
+        <v>5244</v>
       </c>
       <c r="D39" s="11">
-        <v>5673</v>
+        <v>2749</v>
       </c>
       <c r="E39" s="11">
-        <v>4195</v>
+        <v>2026</v>
       </c>
       <c r="F39" s="11">
-        <v>471</v>
+        <v>303</v>
       </c>
       <c r="G39" s="11">
-        <v>906</v>
+        <v>369</v>
       </c>
       <c r="H39" s="11">
-        <v>5572</v>
+        <v>2698</v>
       </c>
       <c r="I39" s="11">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="J39" s="11">
-        <v>7293</v>
+        <v>2495</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C40" s="11">
-        <v>5244</v>
+        <v>406</v>
       </c>
       <c r="D40" s="11">
-        <v>2749</v>
+        <v>406</v>
       </c>
       <c r="E40" s="11">
-        <v>2026</v>
+        <v>309</v>
       </c>
       <c r="F40" s="11">
-        <v>303</v>
+        <v>54</v>
       </c>
       <c r="G40" s="11">
-        <v>369</v>
+        <v>39</v>
       </c>
       <c r="H40" s="11">
-        <v>2698</v>
+        <v>402</v>
       </c>
       <c r="I40" s="11">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="J40" s="11">
-        <v>2495</v>
+        <v>0</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="11">
-        <v>406</v>
+        <v>4838</v>
       </c>
       <c r="D41" s="11">
-        <v>406</v>
+        <v>2343</v>
       </c>
       <c r="E41" s="11">
-        <v>309</v>
+        <v>1717</v>
       </c>
       <c r="F41" s="11">
-        <v>54</v>
+        <v>249</v>
       </c>
       <c r="G41" s="11">
-        <v>39</v>
+        <v>330</v>
       </c>
       <c r="H41" s="11">
-        <v>402</v>
+        <v>2296</v>
       </c>
       <c r="I41" s="11">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="J41" s="11">
-        <v>0</v>
+        <v>2495</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2075,104 +2078,104 @@
         <v>29</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C42" s="11">
-        <v>4838</v>
+        <v>2554</v>
       </c>
       <c r="D42" s="11">
-        <v>2343</v>
+        <v>1265</v>
       </c>
       <c r="E42" s="11">
-        <v>1717</v>
+        <v>769</v>
       </c>
       <c r="F42" s="11">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="G42" s="11">
-        <v>330</v>
+        <v>217</v>
       </c>
       <c r="H42" s="11">
-        <v>2296</v>
+        <v>1239</v>
       </c>
       <c r="I42" s="11">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="J42" s="11">
-        <v>2495</v>
+        <v>1289</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C43" s="11">
-        <v>2554</v>
+        <v>325</v>
       </c>
       <c r="D43" s="11">
-        <v>1265</v>
+        <v>325</v>
       </c>
       <c r="E43" s="11">
-        <v>769</v>
+        <v>197</v>
       </c>
       <c r="F43" s="11">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="G43" s="11">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="H43" s="11">
-        <v>1239</v>
+        <v>317</v>
       </c>
       <c r="I43" s="11">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="J43" s="11">
-        <v>1289</v>
+        <v>0</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C44" s="11">
-        <v>325</v>
+        <v>2229</v>
       </c>
       <c r="D44" s="11">
-        <v>325</v>
+        <v>940</v>
       </c>
       <c r="E44" s="11">
-        <v>197</v>
+        <v>572</v>
       </c>
       <c r="F44" s="11">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="G44" s="11">
-        <v>45</v>
+        <v>172</v>
       </c>
       <c r="H44" s="11">
-        <v>317</v>
+        <v>922</v>
       </c>
       <c r="I44" s="11">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J44" s="11">
-        <v>0</v>
+        <v>1289</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2180,104 +2183,104 @@
         <v>30</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C45" s="11">
-        <v>2229</v>
+        <v>22571</v>
       </c>
       <c r="D45" s="11">
-        <v>940</v>
+        <v>12289</v>
       </c>
       <c r="E45" s="11">
-        <v>572</v>
+        <v>6850</v>
       </c>
       <c r="F45" s="11">
-        <v>178</v>
+        <v>2748</v>
       </c>
       <c r="G45" s="11">
-        <v>172</v>
+        <v>2532</v>
       </c>
       <c r="H45" s="11">
-        <v>922</v>
+        <v>12130</v>
       </c>
       <c r="I45" s="11">
-        <v>18</v>
+        <v>159</v>
       </c>
       <c r="J45" s="11">
-        <v>1289</v>
+        <v>10282</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C46" s="11">
-        <v>22571</v>
+        <v>1814</v>
       </c>
       <c r="D46" s="11">
-        <v>12289</v>
+        <v>1811</v>
       </c>
       <c r="E46" s="11">
-        <v>6850</v>
+        <v>919</v>
       </c>
       <c r="F46" s="11">
-        <v>2748</v>
+        <v>501</v>
       </c>
       <c r="G46" s="11">
-        <v>2532</v>
+        <v>349</v>
       </c>
       <c r="H46" s="11">
-        <v>12130</v>
+        <v>1769</v>
       </c>
       <c r="I46" s="11">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="J46" s="11">
-        <v>10282</v>
+        <v>3</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="11">
-        <v>1814</v>
+        <v>20757</v>
       </c>
       <c r="D47" s="11">
-        <v>1811</v>
+        <v>10478</v>
       </c>
       <c r="E47" s="11">
-        <v>919</v>
+        <v>5931</v>
       </c>
       <c r="F47" s="11">
-        <v>501</v>
+        <v>2247</v>
       </c>
       <c r="G47" s="11">
-        <v>349</v>
+        <v>2183</v>
       </c>
       <c r="H47" s="11">
-        <v>1769</v>
+        <v>10361</v>
       </c>
       <c r="I47" s="11">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="J47" s="11">
-        <v>3</v>
+        <v>10279</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2285,187 +2288,156 @@
         <v>31</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C48" s="11">
-        <v>20757</v>
+        <v>15560</v>
       </c>
       <c r="D48" s="11">
-        <v>10478</v>
+        <v>7402</v>
       </c>
       <c r="E48" s="11">
-        <v>5931</v>
+        <v>4617</v>
       </c>
       <c r="F48" s="11">
-        <v>2247</v>
+        <v>1269</v>
       </c>
       <c r="G48" s="11">
-        <v>2183</v>
+        <v>1438</v>
       </c>
       <c r="H48" s="11">
-        <v>10361</v>
+        <v>7324</v>
       </c>
       <c r="I48" s="11">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="J48" s="11">
-        <v>10279</v>
+        <v>8158</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C49" s="11">
-        <v>15560</v>
+        <v>1149</v>
       </c>
       <c r="D49" s="11">
-        <v>7402</v>
+        <v>1149</v>
       </c>
       <c r="E49" s="11">
-        <v>4617</v>
+        <v>694</v>
       </c>
       <c r="F49" s="11">
-        <v>1269</v>
+        <v>199</v>
       </c>
       <c r="G49" s="11">
-        <v>1438</v>
+        <v>240</v>
       </c>
       <c r="H49" s="11">
-        <v>7324</v>
+        <v>1133</v>
       </c>
       <c r="I49" s="11">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="J49" s="11">
-        <v>8158</v>
+        <v>0</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="11">
-        <v>1149</v>
+        <v>14411</v>
       </c>
       <c r="D50" s="11">
-        <v>1149</v>
+        <v>6253</v>
       </c>
       <c r="E50" s="11">
-        <v>694</v>
+        <v>3923</v>
       </c>
       <c r="F50" s="11">
-        <v>199</v>
+        <v>1070</v>
       </c>
       <c r="G50" s="11">
-        <v>240</v>
+        <v>1198</v>
       </c>
       <c r="H50" s="11">
-        <v>1133</v>
+        <v>6191</v>
       </c>
       <c r="I50" s="11">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="J50" s="11">
+        <v>8158</v>
+      </c>
+      <c r="K50" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="1" customFormat="1">
+      <c r="A51" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="11">
         <v>0</v>
       </c>
-      <c r="K50" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A51" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="11">
-        <v>14411</v>
-      </c>
       <c r="D51" s="11">
-        <v>6253</v>
+        <v>21</v>
       </c>
       <c r="E51" s="11">
-        <v>3923</v>
+        <v>10</v>
       </c>
       <c r="F51" s="11">
-        <v>1070</v>
+        <v>6</v>
       </c>
       <c r="G51" s="11">
-        <v>1198</v>
+        <v>4</v>
       </c>
       <c r="H51" s="11">
-        <v>6191</v>
+        <v>20</v>
       </c>
       <c r="I51" s="11">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="J51" s="11">
-        <v>8158</v>
-      </c>
-      <c r="K51" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" ht="13.5">
-      <c r="A52" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="11">
-        <v>0</v>
-      </c>
-      <c r="D52" s="11">
-        <v>21</v>
-      </c>
-      <c r="E52" s="11">
-        <v>10</v>
-      </c>
-      <c r="F52" s="11">
-        <v>6</v>
-      </c>
-      <c r="G52" s="11">
-        <v>4</v>
-      </c>
-      <c r="H52" s="11">
-        <v>20</v>
-      </c>
-      <c r="I52" s="11">
-        <v>1</v>
-      </c>
-      <c r="J52" s="11">
         <v>-21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
+  <mergeCells count="8">
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>